<commit_message>
Modified Project Charter .xlsx and .doc, Updated ProjectPlan.mpp
</commit_message>
<xml_diff>
--- a/docs/Agile Deliverables Schedule Version 2.3.xlsx
+++ b/docs/Agile Deliverables Schedule Version 2.3.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20353"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Conestoga\PROG8225 - MSD Capstones\New Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afrol\OneDrive\Documents\Capstone\GitHub\easysched\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B71FD9-446A-4795-ABD2-4DF4AE11ADFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC4CE41-C317-4C6E-B80B-EC21CD7CE7F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21972" windowHeight="9774" tabRatio="625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21975" windowHeight="9780" tabRatio="625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Template" sheetId="6" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="62">
   <si>
     <t>Client Sign-off Document</t>
   </si>
@@ -196,15 +196,37 @@
   </si>
   <si>
     <t>Agile Iteration Summary</t>
+  </si>
+  <si>
+    <t>Start of week 6 is Feb 17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start of week 9 is march 9 </t>
+  </si>
+  <si>
+    <t>Start of week 12 is march 30</t>
+  </si>
+  <si>
+    <t>Start of week 13 is April 6</t>
+  </si>
+  <si>
+    <t>Start of week 14 is April 13</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -416,107 +438,108 @@
   </borders>
   <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="33" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="33" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="33" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="33" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="33" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="33" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="33" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="33" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="33" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="33" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="33" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="33" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="35">
     <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
@@ -893,33 +916,33 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.94921875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.94921875" style="3" customWidth="1"/>
-    <col min="3" max="8" width="12.94921875" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.84765625" style="1"/>
+    <col min="1" max="1" width="59" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13" style="3" customWidth="1"/>
+    <col min="3" max="8" width="13" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="29"/>
-    </row>
-    <row r="2" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="30"/>
+    </row>
+    <row r="2" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
       <c r="B2" s="21" t="s">
         <v>43</v>
@@ -943,7 +966,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -954,8 +977,11 @@
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="I3" s="31" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>27</v>
       </c>
@@ -968,8 +994,11 @@
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
       <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="I4" s="31" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
@@ -982,8 +1011,11 @@
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
       <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="I5" s="31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>21</v>
       </c>
@@ -996,8 +1028,11 @@
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="I6" s="31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>41</v>
       </c>
@@ -1010,8 +1045,11 @@
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
       <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="I7" s="31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>42</v>
       </c>
@@ -1025,7 +1063,7 @@
       <c r="G8" s="15"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
@@ -1039,7 +1077,7 @@
       <c r="G9" s="15"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
@@ -1053,7 +1091,7 @@
       <c r="G10" s="15"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>31</v>
       </c>
@@ -1067,7 +1105,7 @@
       <c r="G11" s="15"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>34</v>
       </c>
@@ -1081,7 +1119,7 @@
       <c r="G12" s="15"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>44</v>
       </c>
@@ -1095,7 +1133,7 @@
       <c r="G13" s="15"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
@@ -1107,7 +1145,7 @@
       <c r="G14" s="18"/>
       <c r="H14" s="18"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
         <v>55</v>
       </c>
@@ -1121,7 +1159,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>1</v>
       </c>
@@ -1135,7 +1173,7 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>24</v>
       </c>
@@ -1149,7 +1187,7 @@
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>2</v>
       </c>
@@ -1163,7 +1201,7 @@
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>25</v>
       </c>
@@ -1177,7 +1215,7 @@
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>26</v>
       </c>
@@ -1191,7 +1229,7 @@
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>0</v>
       </c>
@@ -1205,7 +1243,7 @@
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>36</v>
       </c>
@@ -1219,7 +1257,7 @@
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>17</v>
       </c>
@@ -1233,7 +1271,7 @@
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>18</v>
       </c>
@@ -1247,7 +1285,7 @@
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>13</v>
       </c>
@@ -1259,7 +1297,7 @@
       <c r="G25" s="18"/>
       <c r="H25" s="18"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>3</v>
       </c>
@@ -1273,7 +1311,7 @@
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>37</v>
       </c>
@@ -1287,7 +1325,7 @@
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>4</v>
       </c>
@@ -1301,7 +1339,7 @@
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>52</v>
       </c>
@@ -1315,7 +1353,7 @@
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>5</v>
       </c>
@@ -1329,7 +1367,7 @@
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>38</v>
       </c>
@@ -1343,7 +1381,7 @@
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>0</v>
       </c>
@@ -1357,7 +1395,7 @@
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
     </row>
-    <row r="33" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>14</v>
       </c>
@@ -1369,8 +1407,8 @@
       <c r="G33" s="18"/>
       <c r="H33" s="18"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="30" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="27" t="s">
         <v>56</v>
       </c>
       <c r="B34" s="9" t="s">
@@ -1383,7 +1421,7 @@
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>30</v>
       </c>
@@ -1397,7 +1435,7 @@
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>29</v>
       </c>
@@ -1411,7 +1449,7 @@
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
     </row>
-    <row r="37" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>11</v>
       </c>
@@ -1423,7 +1461,7 @@
       <c r="G37" s="12"/>
       <c r="H37" s="18"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>53</v>
       </c>
@@ -1437,7 +1475,7 @@
       <c r="G38" s="13"/>
       <c r="H38" s="5"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>33</v>
       </c>
@@ -1451,7 +1489,7 @@
       <c r="G39" s="13"/>
       <c r="H39" s="5"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>32</v>
       </c>
@@ -1465,7 +1503,7 @@
       <c r="G40" s="13"/>
       <c r="H40" s="5"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>31</v>
       </c>
@@ -1479,7 +1517,7 @@
       <c r="G41" s="13"/>
       <c r="H41" s="5"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>0</v>
       </c>
@@ -1493,7 +1531,7 @@
       <c r="G42" s="13"/>
       <c r="H42" s="5"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>35</v>
       </c>
@@ -1507,7 +1545,7 @@
       <c r="G43" s="13"/>
       <c r="H43" s="5"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>40</v>
       </c>
@@ -1521,7 +1559,7 @@
       <c r="G44" s="13"/>
       <c r="H44" s="5"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>39</v>
       </c>
@@ -1535,7 +1573,7 @@
       <c r="G45" s="13"/>
       <c r="H45" s="5"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>17</v>
       </c>
@@ -1549,7 +1587,7 @@
       <c r="G46" s="13"/>
       <c r="H46" s="5"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>18</v>
       </c>
@@ -1563,7 +1601,7 @@
       <c r="G47" s="13"/>
       <c r="H47" s="5"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>15</v>
       </c>
@@ -1575,7 +1613,7 @@
       <c r="G48" s="14"/>
       <c r="H48" s="23"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>51</v>
       </c>
@@ -1589,7 +1627,7 @@
       <c r="G49" s="15"/>
       <c r="H49" s="24"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>6</v>
       </c>
@@ -1603,7 +1641,7 @@
       <c r="G50" s="15"/>
       <c r="H50" s="24"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>7</v>
       </c>
@@ -1617,7 +1655,7 @@
       <c r="G51" s="15"/>
       <c r="H51" s="24"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>8</v>
       </c>
@@ -1631,7 +1669,7 @@
       <c r="G52" s="15"/>
       <c r="H52" s="24"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>28</v>
       </c>
@@ -1645,7 +1683,7 @@
       <c r="G53" s="15"/>
       <c r="H53" s="24"/>
     </row>
-    <row r="54" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="54" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>9</v>
       </c>

</xml_diff>